<commit_message>
updated list handling of multi-source wells
</commit_message>
<xml_diff>
--- a/source_plates/ECHO_source_plate.xlsx
+++ b/source_plates/ECHO_source_plate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego Alba\Documents\GitHub\WHISPR\source_plates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4C6A44-3E0E-4210-9703-07E4C9F779C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46E3422-4C89-4200-B766-58628B33B3F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{546D7F41-76BF-4117-BD41-03A67E651BAB}"/>
+    <workbookView xWindow="11250" yWindow="5475" windowWidth="20295" windowHeight="14085" xr2:uid="{546D7F41-76BF-4117-BD41-03A67E651BAB}"/>
   </bookViews>
   <sheets>
     <sheet name="ECHO_source_plate" sheetId="1" r:id="rId1"/>
@@ -42,24 +42,6 @@
     <t>Water</t>
   </si>
   <si>
-    <t>A3</t>
-  </si>
-  <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>A5</t>
-  </si>
-  <si>
-    <t>A6</t>
-  </si>
-  <si>
-    <t>A7</t>
-  </si>
-  <si>
-    <t>A8</t>
-  </si>
-  <si>
     <t>Label</t>
   </si>
   <si>
@@ -81,12 +63,6 @@
     <t>Plasmid</t>
   </si>
   <si>
-    <t>A1,A2</t>
-  </si>
-  <si>
-    <t>65,65</t>
-  </si>
-  <si>
     <t>pDA010.188</t>
   </si>
   <si>
@@ -99,25 +75,49 @@
     <t>pRC014</t>
   </si>
   <si>
-    <t>A9</t>
-  </si>
-  <si>
-    <t>A10</t>
-  </si>
-  <si>
     <t>pRC008.206_100x</t>
   </si>
   <si>
     <t>pRC008.206_1000x</t>
   </si>
   <si>
-    <t>A11</t>
-  </si>
-  <si>
     <t>pRC008.206_10000x</t>
   </si>
   <si>
-    <t>A12</t>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>B8</t>
+  </si>
+  <si>
+    <t>B9</t>
+  </si>
+  <si>
+    <t>B11</t>
+  </si>
+  <si>
+    <t>B10</t>
+  </si>
+  <si>
+    <t>B12</t>
+  </si>
+  <si>
+    <t>A1,A2,A3,A4,A5,A6,A7,A8,A9,A10,A11,A12</t>
+  </si>
+  <si>
+    <t>65,65,65,65,65,65,65,65,65,65,65,65</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
   <dimension ref="A1:Y16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,19 +504,19 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -547,11 +547,11 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -582,7 +582,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1">
         <v>150</v>
@@ -616,10 +616,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1">
         <v>1.5</v>
@@ -653,10 +653,10 @@
         <v>0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <v>0.15</v>
@@ -687,13 +687,13 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1">
         <v>199.76</v>
@@ -724,13 +724,13 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1">
         <v>201.96</v>
@@ -761,13 +761,13 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1">
         <v>164.65</v>
@@ -798,13 +798,13 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D9" s="1">
         <v>126.77</v>
@@ -835,53 +835,33 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="D10" s="1">
-        <v>0.16464999999999999</v>
+        <v>16.465</v>
       </c>
       <c r="E10" s="3">
         <v>50</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="D11" s="1">
-        <v>16.465</v>
+        <v>0.16464999999999999</v>
       </c>
       <c r="E11" s="3">
         <v>50</v>
@@ -909,13 +889,13 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1">
         <v>1.6465E-2</v>
@@ -945,10 +925,6 @@
       <c r="Y12" s="1"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>

</xml_diff>